<commit_message>
parser and 2 templates
</commit_message>
<xml_diff>
--- a/app/static/user_data/Keywords.xlsx
+++ b/app/static/user_data/Keywords.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="15620"/>
+    <workbookView xWindow="14060" yWindow="420" windowWidth="24000" windowHeight="15620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="287">
   <si>
     <t>{last_name}</t>
   </si>
@@ -808,6 +808,78 @@
   </si>
   <si>
     <t>Последние 2 цифры года рождения</t>
+  </si>
+  <si>
+    <t>Служебные данные</t>
+  </si>
+  <si>
+    <t>{personal_number}</t>
+  </si>
+  <si>
+    <t>{voin_chast}</t>
+  </si>
+  <si>
+    <t>{prisyaga_date}</t>
+  </si>
+  <si>
+    <t>Личный номер</t>
+  </si>
+  <si>
+    <t>Воинская часть</t>
+  </si>
+  <si>
+    <t>Дата принятия присяги</t>
+  </si>
+  <si>
+    <t>{chislo@prisyaga_date}</t>
+  </si>
+  <si>
+    <t>{month@prisyaga_date}</t>
+  </si>
+  <si>
+    <t>{year@prisyaga_date}</t>
+  </si>
+  <si>
+    <t>Число принятия присяги</t>
+  </si>
+  <si>
+    <t>Месяц принятия присяги</t>
+  </si>
+  <si>
+    <t>Год принятия присяги</t>
+  </si>
+  <si>
+    <t>Прочее</t>
+  </si>
+  <si>
+    <t>{generation_date}</t>
+  </si>
+  <si>
+    <t>{chislo@generation_date}</t>
+  </si>
+  <si>
+    <t>{month@generation_date}</t>
+  </si>
+  <si>
+    <t>{year@generation_date}</t>
+  </si>
+  <si>
+    <t>Дата документа</t>
+  </si>
+  <si>
+    <t>Число</t>
+  </si>
+  <si>
+    <t>Месяц</t>
+  </si>
+  <si>
+    <t>Год</t>
+  </si>
+  <si>
+    <t>{year_last2@generation_date}</t>
+  </si>
+  <si>
+    <t>Последние 2 цифры года</t>
   </si>
 </sst>
 </file>
@@ -922,7 +994,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -931,8 +1003,24 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -953,10 +1041,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -975,15 +1059,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="24">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1313,10 +1416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F183"/>
+  <dimension ref="A1:F196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="B196" sqref="B196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1326,69 +1429,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="23">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="23" customHeight="1">
-      <c r="A2" s="15"/>
+      <c r="A2" s="13"/>
     </row>
     <row r="3" spans="1:1" ht="23" customHeight="1">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="13" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="23">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="13" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="23">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="13" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="23">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="13" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="23">
-      <c r="A7" s="15"/>
+      <c r="A7" s="13"/>
     </row>
     <row r="8" spans="1:1" ht="23">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="13" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="23">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="13" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="23">
-      <c r="A10" s="15"/>
+      <c r="A10" s="13"/>
     </row>
     <row r="11" spans="1:1" ht="23">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="13" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="23">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="13" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="23">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="13" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="23">
-      <c r="A14" s="15"/>
+      <c r="A14" s="13"/>
     </row>
     <row r="15" spans="1:1" ht="23">
-      <c r="A15" s="15"/>
+      <c r="A15" s="13"/>
     </row>
     <row r="17" spans="1:6" ht="20" thickBot="1">
       <c r="A17" s="3" t="s">
@@ -2344,564 +2447,673 @@
         <v>233</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="19">
-      <c r="A133" s="10" t="s">
+    <row r="133" spans="1:6" ht="20" thickBot="1">
+      <c r="A133" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B133" s="3"/>
+      <c r="C133" s="3"/>
+      <c r="D133" s="3"/>
+      <c r="E133" s="3"/>
+      <c r="F133" s="3"/>
+    </row>
+    <row r="134" spans="1:6" ht="16" thickTop="1">
+      <c r="A134" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B134" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
+      <c r="A135" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B135" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
+      <c r="A136" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B136" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
+      <c r="A137" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B137" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
+      <c r="A138" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B138" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
+      <c r="A139" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B139" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" ht="20" thickBot="1">
+      <c r="A140" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B133" s="11"/>
-      <c r="C133" s="11"/>
-      <c r="D133" s="11"/>
-      <c r="E133" s="11"/>
-      <c r="F133" s="11"/>
-    </row>
-    <row r="134" spans="1:6">
-      <c r="A134" s="12" t="s">
+      <c r="B140" s="3"/>
+      <c r="C140" s="3"/>
+      <c r="D140" s="3"/>
+      <c r="E140" s="3"/>
+      <c r="F140" s="3"/>
+    </row>
+    <row r="141" spans="1:6" ht="16" thickTop="1">
+      <c r="A141" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="B134" s="13" t="s">
+      <c r="B141" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="C134" s="16" t="s">
+      <c r="C141" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="D134" s="16"/>
-      <c r="E134" s="13"/>
-      <c r="F134" s="13"/>
-    </row>
-    <row r="135" spans="1:6">
-      <c r="A135" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B135" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="C135" s="17"/>
-      <c r="D135" s="17"/>
-      <c r="E135" s="7"/>
-      <c r="F135" s="7"/>
-    </row>
-    <row r="136" spans="1:6">
-      <c r="A136" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B136" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="C136" s="17"/>
-      <c r="D136" s="17"/>
-      <c r="E136" s="7"/>
-      <c r="F136" s="7"/>
-    </row>
-    <row r="137" spans="1:6">
-      <c r="A137" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="B137" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="C137" s="17"/>
-      <c r="D137" s="17"/>
-      <c r="E137" s="7"/>
-      <c r="F137" s="7"/>
-    </row>
-    <row r="138" spans="1:6">
-      <c r="A138" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B138" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="C138" s="17"/>
-      <c r="D138" s="17"/>
-      <c r="E138" s="7"/>
-      <c r="F138" s="7"/>
-    </row>
-    <row r="139" spans="1:6">
-      <c r="A139" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B139" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="C139" s="17"/>
-      <c r="D139" s="17"/>
-      <c r="E139" s="7"/>
-      <c r="F139" s="7"/>
-    </row>
-    <row r="140" spans="1:6">
-      <c r="A140" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B140" s="14" t="s">
-        <v>216</v>
-      </c>
-      <c r="C140" s="17"/>
-      <c r="D140" s="17"/>
-      <c r="E140" s="7"/>
-      <c r="F140" s="7"/>
-    </row>
-    <row r="141" spans="1:6">
-      <c r="A141" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="B141" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="C141" s="17"/>
-      <c r="D141" s="17"/>
-      <c r="E141" s="7"/>
-      <c r="F141" s="7"/>
+      <c r="D141" s="14"/>
+      <c r="E141" s="11"/>
+      <c r="F141" s="11"/>
     </row>
     <row r="142" spans="1:6">
       <c r="A142" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B142" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="C142" s="17"/>
-      <c r="D142" s="17"/>
+        <v>98</v>
+      </c>
+      <c r="B142" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="C142" s="15"/>
+      <c r="D142" s="15"/>
       <c r="E142" s="7"/>
       <c r="F142" s="7"/>
     </row>
     <row r="143" spans="1:6">
       <c r="A143" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="B143" s="14" t="s">
-        <v>218</v>
-      </c>
-      <c r="C143" s="17"/>
-      <c r="D143" s="17"/>
+        <v>99</v>
+      </c>
+      <c r="B143" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C143" s="15"/>
+      <c r="D143" s="15"/>
       <c r="E143" s="7"/>
       <c r="F143" s="7"/>
     </row>
     <row r="144" spans="1:6">
       <c r="A144" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B144" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="C144" s="17"/>
-      <c r="D144" s="17"/>
+        <v>100</v>
+      </c>
+      <c r="B144" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C144" s="15"/>
+      <c r="D144" s="15"/>
       <c r="E144" s="7"/>
       <c r="F144" s="7"/>
     </row>
     <row r="145" spans="1:6">
       <c r="A145" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B145" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C145" s="17"/>
-      <c r="D145" s="17"/>
+        <v>101</v>
+      </c>
+      <c r="B145" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C145" s="15"/>
+      <c r="D145" s="15"/>
       <c r="E145" s="7"/>
       <c r="F145" s="7"/>
     </row>
     <row r="146" spans="1:6">
       <c r="A146" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B146" s="14" t="s">
-        <v>235</v>
-      </c>
-      <c r="C146" s="17"/>
-      <c r="D146" s="17"/>
+        <v>102</v>
+      </c>
+      <c r="B146" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="C146" s="15"/>
+      <c r="D146" s="15"/>
       <c r="E146" s="7"/>
       <c r="F146" s="7"/>
     </row>
     <row r="147" spans="1:6">
-      <c r="A147" s="8" t="s">
+      <c r="A147" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B147" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="C147" s="15"/>
+      <c r="D147" s="15"/>
+      <c r="E147" s="7"/>
+      <c r="F147" s="7"/>
+    </row>
+    <row r="148" spans="1:6">
+      <c r="A148" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B148" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="C148" s="15"/>
+      <c r="D148" s="15"/>
+      <c r="E148" s="7"/>
+      <c r="F148" s="7"/>
+    </row>
+    <row r="149" spans="1:6">
+      <c r="A149" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B149" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="C149" s="15"/>
+      <c r="D149" s="15"/>
+      <c r="E149" s="7"/>
+      <c r="F149" s="7"/>
+    </row>
+    <row r="150" spans="1:6">
+      <c r="A150" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B150" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="C150" s="15"/>
+      <c r="D150" s="15"/>
+      <c r="E150" s="7"/>
+      <c r="F150" s="7"/>
+    </row>
+    <row r="151" spans="1:6">
+      <c r="A151" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B151" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="C151" s="15"/>
+      <c r="D151" s="15"/>
+      <c r="E151" s="7"/>
+      <c r="F151" s="7"/>
+    </row>
+    <row r="152" spans="1:6">
+      <c r="A152" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B152" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="C152" s="15"/>
+      <c r="D152" s="15"/>
+      <c r="E152" s="7"/>
+      <c r="F152" s="7"/>
+    </row>
+    <row r="153" spans="1:6">
+      <c r="A153" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B153" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="C153" s="15"/>
+      <c r="D153" s="15"/>
+      <c r="E153" s="7"/>
+      <c r="F153" s="7"/>
+    </row>
+    <row r="154" spans="1:6">
+      <c r="A154" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B147" s="9" t="s">
+      <c r="B154" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="C147" s="18"/>
-      <c r="D147" s="18"/>
-      <c r="E147" s="9"/>
-      <c r="F147" s="9"/>
-    </row>
-    <row r="148" spans="1:6">
-      <c r="A148" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B148" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="C148" s="16" t="s">
-        <v>237</v>
-      </c>
-      <c r="D148" s="16"/>
-    </row>
-    <row r="149" spans="1:6">
-      <c r="A149" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B149" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="C149" s="17"/>
-      <c r="D149" s="17"/>
-    </row>
-    <row r="150" spans="1:6">
-      <c r="A150" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B150" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="C150" s="17"/>
-      <c r="D150" s="17"/>
-    </row>
-    <row r="151" spans="1:6">
-      <c r="A151" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B151" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="C151" s="17"/>
-      <c r="D151" s="17"/>
-    </row>
-    <row r="152" spans="1:6">
-      <c r="A152" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B152" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="C152" s="17"/>
-      <c r="D152" s="17"/>
-    </row>
-    <row r="153" spans="1:6">
-      <c r="A153" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B153" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="C153" s="17"/>
-      <c r="D153" s="17"/>
-    </row>
-    <row r="154" spans="1:6">
-      <c r="A154" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B154" s="14" t="s">
-        <v>216</v>
-      </c>
-      <c r="C154" s="17"/>
-      <c r="D154" s="17"/>
+      <c r="C154" s="16"/>
+      <c r="D154" s="16"/>
+      <c r="E154" s="9"/>
+      <c r="F154" s="9"/>
     </row>
     <row r="155" spans="1:6">
       <c r="A155" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B155" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="C155" s="17"/>
-      <c r="D155" s="17"/>
+        <v>111</v>
+      </c>
+      <c r="B155" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="C155" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="D155" s="14"/>
     </row>
     <row r="156" spans="1:6">
       <c r="A156" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B156" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="C156" s="17"/>
-      <c r="D156" s="17"/>
+        <v>112</v>
+      </c>
+      <c r="B156" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="C156" s="15"/>
+      <c r="D156" s="15"/>
     </row>
     <row r="157" spans="1:6">
       <c r="A157" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B157" s="14" t="s">
-        <v>218</v>
-      </c>
-      <c r="C157" s="17"/>
-      <c r="D157" s="17"/>
+        <v>113</v>
+      </c>
+      <c r="B157" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C157" s="15"/>
+      <c r="D157" s="15"/>
     </row>
     <row r="158" spans="1:6">
       <c r="A158" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B158" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="C158" s="17"/>
-      <c r="D158" s="17"/>
+        <v>114</v>
+      </c>
+      <c r="B158" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C158" s="15"/>
+      <c r="D158" s="15"/>
     </row>
     <row r="159" spans="1:6">
       <c r="A159" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B159" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C159" s="17"/>
-      <c r="D159" s="17"/>
+        <v>115</v>
+      </c>
+      <c r="B159" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C159" s="15"/>
+      <c r="D159" s="15"/>
     </row>
     <row r="160" spans="1:6">
       <c r="A160" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B160" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="C160" s="15"/>
+      <c r="D160" s="15"/>
+    </row>
+    <row r="161" spans="1:6">
+      <c r="A161" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B161" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="C161" s="15"/>
+      <c r="D161" s="15"/>
+    </row>
+    <row r="162" spans="1:6">
+      <c r="A162" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B162" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="C162" s="15"/>
+      <c r="D162" s="15"/>
+    </row>
+    <row r="163" spans="1:6">
+      <c r="A163" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B163" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="C163" s="15"/>
+      <c r="D163" s="15"/>
+    </row>
+    <row r="164" spans="1:6">
+      <c r="A164" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B164" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="C164" s="15"/>
+      <c r="D164" s="15"/>
+    </row>
+    <row r="165" spans="1:6">
+      <c r="A165" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B165" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="C165" s="15"/>
+      <c r="D165" s="15"/>
+    </row>
+    <row r="166" spans="1:6">
+      <c r="A166" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B166" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="C166" s="15"/>
+      <c r="D166" s="15"/>
+    </row>
+    <row r="167" spans="1:6">
+      <c r="A167" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B160" s="14" t="s">
+      <c r="B167" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="C160" s="17"/>
-      <c r="D160" s="17"/>
-    </row>
-    <row r="161" spans="1:6">
-      <c r="A161" s="8" t="s">
+      <c r="C167" s="15"/>
+      <c r="D167" s="15"/>
+    </row>
+    <row r="168" spans="1:6">
+      <c r="A168" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="B161" s="9" t="s">
+      <c r="B168" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="C161" s="18"/>
-      <c r="D161" s="18"/>
-    </row>
-    <row r="162" spans="1:6" ht="20" thickBot="1">
-      <c r="A162" s="2" t="s">
+      <c r="C168" s="16"/>
+      <c r="D168" s="16"/>
+    </row>
+    <row r="169" spans="1:6" ht="20" thickBot="1">
+      <c r="A169" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B162" s="3"/>
-      <c r="C162" s="3"/>
-      <c r="D162" s="3"/>
-      <c r="E162" s="3"/>
-      <c r="F162" s="3"/>
-    </row>
-    <row r="163" spans="1:6" ht="16" thickTop="1">
-      <c r="A163" s="4" t="s">
+      <c r="B169" s="3"/>
+      <c r="C169" s="3"/>
+      <c r="D169" s="3"/>
+      <c r="E169" s="3"/>
+      <c r="F169" s="3"/>
+    </row>
+    <row r="170" spans="1:6" ht="16" thickTop="1">
+      <c r="A170" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B163" s="5" t="s">
+      <c r="B170" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="C163" s="19" t="s">
+      <c r="C170" s="17" t="s">
         <v>238</v>
       </c>
-      <c r="D163" s="19"/>
-    </row>
-    <row r="164" spans="1:6">
-      <c r="A164" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="B164" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="C164" s="17"/>
-      <c r="D164" s="17"/>
-    </row>
-    <row r="165" spans="1:6">
-      <c r="A165" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="B165" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="C165" s="17"/>
-      <c r="D165" s="17"/>
-    </row>
-    <row r="166" spans="1:6">
-      <c r="A166" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="B166" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="C166" s="17"/>
-      <c r="D166" s="17"/>
-    </row>
-    <row r="167" spans="1:6">
-      <c r="A167" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="B167" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="C167" s="17"/>
-      <c r="D167" s="17"/>
-    </row>
-    <row r="168" spans="1:6">
-      <c r="A168" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="B168" s="14" t="s">
-        <v>235</v>
-      </c>
-      <c r="C168" s="17"/>
-      <c r="D168" s="17"/>
-    </row>
-    <row r="169" spans="1:6">
-      <c r="A169" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="B169" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="C169" s="18"/>
-      <c r="D169" s="18"/>
-    </row>
-    <row r="170" spans="1:6">
-      <c r="A170" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="B170" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="C170" s="16" t="s">
-        <v>239</v>
-      </c>
-      <c r="D170" s="16"/>
+      <c r="D170" s="17"/>
     </row>
     <row r="171" spans="1:6">
       <c r="A171" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="B171" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B171" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="C171" s="17"/>
-      <c r="D171" s="17"/>
+      <c r="C171" s="15"/>
+      <c r="D171" s="15"/>
     </row>
     <row r="172" spans="1:6">
       <c r="A172" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="B172" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B172" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="C172" s="17"/>
-      <c r="D172" s="17"/>
+      <c r="C172" s="15"/>
+      <c r="D172" s="15"/>
     </row>
     <row r="173" spans="1:6">
       <c r="A173" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="B173" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B173" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="C173" s="17"/>
-      <c r="D173" s="17"/>
+      <c r="C173" s="15"/>
+      <c r="D173" s="15"/>
     </row>
     <row r="174" spans="1:6">
       <c r="A174" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="B174" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B174" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="C174" s="17"/>
-      <c r="D174" s="17"/>
+      <c r="C174" s="15"/>
+      <c r="D174" s="15"/>
     </row>
     <row r="175" spans="1:6">
       <c r="A175" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="B175" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B175" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="C175" s="17"/>
-      <c r="D175" s="17"/>
+      <c r="C175" s="15"/>
+      <c r="D175" s="15"/>
     </row>
     <row r="176" spans="1:6">
       <c r="A176" s="8" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B176" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="C176" s="18"/>
-      <c r="D176" s="18"/>
-    </row>
-    <row r="177" spans="1:4">
-      <c r="A177" s="6" t="s">
-        <v>139</v>
+      <c r="C176" s="16"/>
+      <c r="D176" s="16"/>
+    </row>
+    <row r="177" spans="1:6">
+      <c r="A177" s="10" t="s">
+        <v>132</v>
       </c>
       <c r="B177" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="C177" s="17" t="s">
-        <v>240</v>
-      </c>
-      <c r="D177" s="17"/>
-    </row>
-    <row r="178" spans="1:4">
+      <c r="C177" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="D177" s="14"/>
+    </row>
+    <row r="178" spans="1:6">
       <c r="A178" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="B178" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B178" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="C178" s="17"/>
-      <c r="D178" s="17"/>
-    </row>
-    <row r="179" spans="1:4">
+      <c r="C178" s="15"/>
+      <c r="D178" s="15"/>
+    </row>
+    <row r="179" spans="1:6">
       <c r="A179" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="B179" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="B179" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="C179" s="17"/>
-      <c r="D179" s="17"/>
-    </row>
-    <row r="180" spans="1:4">
+      <c r="C179" s="15"/>
+      <c r="D179" s="15"/>
+    </row>
+    <row r="180" spans="1:6">
       <c r="A180" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="B180" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B180" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="C180" s="17"/>
-      <c r="D180" s="17"/>
-    </row>
-    <row r="181" spans="1:4">
+      <c r="C180" s="15"/>
+      <c r="D180" s="15"/>
+    </row>
+    <row r="181" spans="1:6">
       <c r="A181" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="B181" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B181" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="C181" s="17"/>
-      <c r="D181" s="17"/>
-    </row>
-    <row r="182" spans="1:4">
+      <c r="C181" s="15"/>
+      <c r="D181" s="15"/>
+    </row>
+    <row r="182" spans="1:6">
       <c r="A182" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="B182" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B182" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="C182" s="17"/>
-      <c r="D182" s="17"/>
-    </row>
-    <row r="183" spans="1:4">
+      <c r="C182" s="15"/>
+      <c r="D182" s="15"/>
+    </row>
+    <row r="183" spans="1:6">
       <c r="A183" s="8" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B183" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="C183" s="18"/>
-      <c r="D183" s="18"/>
+      <c r="C183" s="16"/>
+      <c r="D183" s="16"/>
+    </row>
+    <row r="184" spans="1:6">
+      <c r="A184" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B184" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C184" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="D184" s="15"/>
+    </row>
+    <row r="185" spans="1:6">
+      <c r="A185" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B185" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="C185" s="15"/>
+      <c r="D185" s="15"/>
+    </row>
+    <row r="186" spans="1:6">
+      <c r="A186" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B186" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C186" s="15"/>
+      <c r="D186" s="15"/>
+    </row>
+    <row r="187" spans="1:6">
+      <c r="A187" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B187" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C187" s="15"/>
+      <c r="D187" s="15"/>
+    </row>
+    <row r="188" spans="1:6">
+      <c r="A188" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B188" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C188" s="15"/>
+      <c r="D188" s="15"/>
+    </row>
+    <row r="189" spans="1:6">
+      <c r="A189" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B189" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="C189" s="15"/>
+      <c r="D189" s="15"/>
+    </row>
+    <row r="190" spans="1:6">
+      <c r="A190" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B190" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="C190" s="16"/>
+      <c r="D190" s="16"/>
+    </row>
+    <row r="191" spans="1:6" ht="20" thickBot="1">
+      <c r="A191" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="B191" s="3"/>
+      <c r="C191" s="3"/>
+      <c r="D191" s="3"/>
+      <c r="E191" s="3"/>
+      <c r="F191" s="3"/>
+    </row>
+    <row r="192" spans="1:6" ht="16" thickTop="1">
+      <c r="A192" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="B192" s="12" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2">
+      <c r="A193" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="B193" s="12" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2">
+      <c r="A194" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="B194" s="12" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2">
+      <c r="A195" s="18" t="s">
+        <v>280</v>
+      </c>
+      <c r="B195" s="12" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2">
+      <c r="A196" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="B196" s="12" t="s">
+        <v>286</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="C134:D147"/>
-    <mergeCell ref="C148:D161"/>
-    <mergeCell ref="C163:D169"/>
+    <mergeCell ref="C141:D154"/>
+    <mergeCell ref="C155:D168"/>
     <mergeCell ref="C170:D176"/>
     <mergeCell ref="C177:D183"/>
+    <mergeCell ref="C184:D190"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>